<commit_message>
Actualización completa del sistema de asistencia QR
</commit_message>
<xml_diff>
--- a/static/reporte_asistencia.xlsx
+++ b/static/reporte_asistencia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,84 +436,168 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ID Empleado</t>
+          <t>Fecha</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Departamento</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Fecha</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Hora</t>
+          <t>Entrada</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Tipo</t>
+          <t>Salida</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Latitud</t>
+          <t>Horas Trabajadas</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Longitud</t>
+          <t>Dirección</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EMP006</t>
+          <t>11/08/2025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Yadira  Zeballos </t>
+          <t>E001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ventas</t>
+          <t>Yadira Zeballos</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>27/07/2025</t>
+          <t xml:space="preserve">Tecnologia Digital </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>22:10:24</t>
+          <t>09:34:51</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Entrada</t>
+          <t>10:33:02</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>58 minutos, 11 segundos</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Institución Educativa No. 40657, Elías Aguirre, Selva Alegre, Chilina, Alto Selva Alegre, Arequipa, 04003, Perú</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>11/08/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>E002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Melani Zeballos </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>09:54:38</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>No registrada</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Institución Educativa No. 40657, Elías Aguirre, Selva Alegre, Chilina, Alto Selva Alegre, Arequipa, 04003, Perú</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>11/08/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>E003</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Luis Lopez</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tecnologia Digital </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>10:33:13</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>20:33:34</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>10 horas, 21 segundos</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Institución Educativa No. 40657, Elías Aguirre, Selva Alegre, Chilina, Alto Selva Alegre, Arequipa, 04003, Perú</t>
         </is>
       </c>
     </row>

</xml_diff>